<commit_message>
Update Binding Conservation sample input
General update to all codes and readme's
</commit_message>
<xml_diff>
--- a/2_bindingAnalysis/sampleInputs/C_USP9x.xlsx
+++ b/2_bindingAnalysis/sampleInputs/C_USP9x.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhang elitebook\Documents\Olivia\pdEmma\clean\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spyro\Work\zhangLab\scripts\python\phageDisplayAnalysis\2_bindingAnalysis\sampleInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0C42515-2F05-4D27-BBA0-671B3E944F59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DD7686-BB77-4F29-B7E8-4D9A04C1F218}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10590"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plate 1 - Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="239">
   <si>
     <t>Software Version</t>
   </si>
@@ -463,13 +463,298 @@
     <t>Actual Temperature:</t>
   </si>
   <si>
-    <t>Normalized Absorbance</t>
+    <t>CTRL1</t>
+  </si>
+  <si>
+    <t>CTRL2</t>
+  </si>
+  <si>
+    <t>CTRL3</t>
+  </si>
+  <si>
+    <t>CTRL4</t>
+  </si>
+  <si>
+    <t>CTRL5</t>
+  </si>
+  <si>
+    <t>CTRL6</t>
+  </si>
+  <si>
+    <t>CTRL7</t>
+  </si>
+  <si>
+    <t>CTRL8</t>
+  </si>
+  <si>
+    <t>CTRL9</t>
+  </si>
+  <si>
+    <t>CTRL10</t>
+  </si>
+  <si>
+    <t>CTRL11</t>
+  </si>
+  <si>
+    <t>CTRL12</t>
+  </si>
+  <si>
+    <t>CTRL13</t>
+  </si>
+  <si>
+    <t>CTRL14</t>
+  </si>
+  <si>
+    <t>CTRL15</t>
+  </si>
+  <si>
+    <t>CTRL16</t>
+  </si>
+  <si>
+    <t>CTRL17</t>
+  </si>
+  <si>
+    <t>CTRL18</t>
+  </si>
+  <si>
+    <t>CTRL19</t>
+  </si>
+  <si>
+    <t>CTRL20</t>
+  </si>
+  <si>
+    <t>CTRL21</t>
+  </si>
+  <si>
+    <t>CTRL22</t>
+  </si>
+  <si>
+    <t>CTRL23</t>
+  </si>
+  <si>
+    <t>CTRL24</t>
+  </si>
+  <si>
+    <t>CTRL25</t>
+  </si>
+  <si>
+    <t>CTRL26</t>
+  </si>
+  <si>
+    <t>CTRL27</t>
+  </si>
+  <si>
+    <t>CTRL28</t>
+  </si>
+  <si>
+    <t>CTRL29</t>
+  </si>
+  <si>
+    <t>CTRL30</t>
+  </si>
+  <si>
+    <t>CTRL31</t>
+  </si>
+  <si>
+    <t>CTRL32</t>
+  </si>
+  <si>
+    <t>CTRL33</t>
+  </si>
+  <si>
+    <t>CTRL34</t>
+  </si>
+  <si>
+    <t>CTRL35</t>
+  </si>
+  <si>
+    <t>CTRL36</t>
+  </si>
+  <si>
+    <t>CTRL37</t>
+  </si>
+  <si>
+    <t>CTRL38</t>
+  </si>
+  <si>
+    <t>CTRL39</t>
+  </si>
+  <si>
+    <t>CTRL40</t>
+  </si>
+  <si>
+    <t>CTRL41</t>
+  </si>
+  <si>
+    <t>CTRL42</t>
+  </si>
+  <si>
+    <t>CTRL43</t>
+  </si>
+  <si>
+    <t>CTRL44</t>
+  </si>
+  <si>
+    <t>CTRL45</t>
+  </si>
+  <si>
+    <t>CTRL46</t>
+  </si>
+  <si>
+    <t>CTRL47</t>
+  </si>
+  <si>
+    <t>CTRL48</t>
+  </si>
+  <si>
+    <t>CTRL49</t>
+  </si>
+  <si>
+    <t>CTRL50</t>
+  </si>
+  <si>
+    <t>CTRL51</t>
+  </si>
+  <si>
+    <t>CTRL52</t>
+  </si>
+  <si>
+    <t>CTRL53</t>
+  </si>
+  <si>
+    <t>CTRL54</t>
+  </si>
+  <si>
+    <t>CTRL55</t>
+  </si>
+  <si>
+    <t>CTRL56</t>
+  </si>
+  <si>
+    <t>CTRL57</t>
+  </si>
+  <si>
+    <t>CTRL58</t>
+  </si>
+  <si>
+    <t>CTRL59</t>
+  </si>
+  <si>
+    <t>CTRL60</t>
+  </si>
+  <si>
+    <t>CTRL61</t>
+  </si>
+  <si>
+    <t>CTRL62</t>
+  </si>
+  <si>
+    <t>CTRL63</t>
+  </si>
+  <si>
+    <t>CTRL64</t>
+  </si>
+  <si>
+    <t>CTRL65</t>
+  </si>
+  <si>
+    <t>CTRL66</t>
+  </si>
+  <si>
+    <t>CTRL67</t>
+  </si>
+  <si>
+    <t>CTRL68</t>
+  </si>
+  <si>
+    <t>CTRL69</t>
+  </si>
+  <si>
+    <t>CTRL70</t>
+  </si>
+  <si>
+    <t>CTRL71</t>
+  </si>
+  <si>
+    <t>CTRL72</t>
+  </si>
+  <si>
+    <t>CTRL73</t>
+  </si>
+  <si>
+    <t>CTRL74</t>
+  </si>
+  <si>
+    <t>CTRL75</t>
+  </si>
+  <si>
+    <t>CTRL76</t>
+  </si>
+  <si>
+    <t>CTRL77</t>
+  </si>
+  <si>
+    <t>CTRL78</t>
+  </si>
+  <si>
+    <t>CTRL79</t>
+  </si>
+  <si>
+    <t>CTRL80</t>
+  </si>
+  <si>
+    <t>CTRL81</t>
+  </si>
+  <si>
+    <t>CTRL82</t>
+  </si>
+  <si>
+    <t>CTRL83</t>
+  </si>
+  <si>
+    <t>CTRL84</t>
+  </si>
+  <si>
+    <t>CTRL85</t>
+  </si>
+  <si>
+    <t>CTRL86</t>
+  </si>
+  <si>
+    <t>CTRL87</t>
+  </si>
+  <si>
+    <t>CTRL88</t>
+  </si>
+  <si>
+    <t>CTRL89</t>
+  </si>
+  <si>
+    <t>CTRL90</t>
+  </si>
+  <si>
+    <t>CTRL91</t>
+  </si>
+  <si>
+    <t>CTRL92</t>
+  </si>
+  <si>
+    <t>CTRL93</t>
+  </si>
+  <si>
+    <t>CTRL94</t>
+  </si>
+  <si>
+    <t>CTRL95</t>
+  </si>
+  <si>
+    <t>CTRL96</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -502,7 +787,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -617,6 +902,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -715,7 +1006,7 @@
     <xf numFmtId="0" fontId="2" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1031,11 +1322,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AA82"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:AA62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="AE80" sqref="AE80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1336,30 +1627,78 @@
       <c r="B27" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
-      <c r="U27" s="9"/>
-      <c r="V27" s="9"/>
-      <c r="W27" s="9"/>
-      <c r="X27" s="9"/>
-      <c r="Y27" s="9"/>
-      <c r="Z27" s="9"/>
+      <c r="C27" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="J27" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="K27" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="L27" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="M27" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="N27" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="O27" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="P27" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q27" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="R27" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="S27" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="T27" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="U27" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="V27" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="W27" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="X27" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y27" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z27" s="25" t="s">
+        <v>154</v>
+      </c>
       <c r="AA27" s="8" t="s">
         <v>41</v>
       </c>
@@ -1448,30 +1787,78 @@
       <c r="B29" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
-      <c r="U29" s="9"/>
-      <c r="V29" s="9"/>
-      <c r="W29" s="9"/>
-      <c r="X29" s="9"/>
-      <c r="Y29" s="9"/>
-      <c r="Z29" s="9"/>
+      <c r="C29" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="J29" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="L29" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="M29" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="N29" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="O29" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="P29" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q29" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="R29" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="S29" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="T29" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="U29" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="V29" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="W29" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="X29" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y29" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z29" s="25" t="s">
+        <v>166</v>
+      </c>
       <c r="AA29" s="8" t="s">
         <v>41</v>
       </c>
@@ -1560,30 +1947,78 @@
       <c r="B31" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
-      <c r="R31" s="9"/>
-      <c r="S31" s="9"/>
-      <c r="T31" s="9"/>
-      <c r="U31" s="9"/>
-      <c r="V31" s="9"/>
-      <c r="W31" s="9"/>
-      <c r="X31" s="9"/>
-      <c r="Y31" s="9"/>
-      <c r="Z31" s="9"/>
+      <c r="C31" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H31" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="J31" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="K31" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="L31" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="M31" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="N31" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="O31" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="P31" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q31" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="R31" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="S31" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="T31" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="U31" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="V31" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="W31" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="X31" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="Y31" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z31" s="25" t="s">
+        <v>178</v>
+      </c>
       <c r="AA31" s="8" t="s">
         <v>41</v>
       </c>
@@ -1672,30 +2107,78 @@
       <c r="B33" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="9"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="9"/>
-      <c r="R33" s="9"/>
-      <c r="S33" s="9"/>
-      <c r="T33" s="9"/>
-      <c r="U33" s="9"/>
-      <c r="V33" s="9"/>
-      <c r="W33" s="9"/>
-      <c r="X33" s="9"/>
-      <c r="Y33" s="9"/>
-      <c r="Z33" s="9"/>
+      <c r="C33" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F33" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H33" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="J33" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="K33" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="L33" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="M33" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="N33" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="O33" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="P33" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q33" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="R33" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="S33" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="T33" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="U33" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="V33" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="W33" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="X33" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y33" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z33" s="25" t="s">
+        <v>190</v>
+      </c>
       <c r="AA33" s="8" t="s">
         <v>41</v>
       </c>
@@ -1784,30 +2267,78 @@
       <c r="B35" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="9"/>
-      <c r="R35" s="9"/>
-      <c r="S35" s="9"/>
-      <c r="T35" s="9"/>
-      <c r="U35" s="9"/>
-      <c r="V35" s="9"/>
-      <c r="W35" s="9"/>
-      <c r="X35" s="9"/>
-      <c r="Y35" s="9"/>
-      <c r="Z35" s="9"/>
+      <c r="C35" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F35" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H35" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="J35" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="K35" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="L35" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="M35" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="N35" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="O35" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="P35" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q35" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="R35" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="S35" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="T35" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="U35" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="V35" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="W35" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="X35" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="Y35" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z35" s="25" t="s">
+        <v>202</v>
+      </c>
       <c r="AA35" s="8" t="s">
         <v>41</v>
       </c>
@@ -1896,30 +2427,78 @@
       <c r="B37" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
-      <c r="O37" s="9"/>
-      <c r="P37" s="9"/>
-      <c r="Q37" s="9"/>
-      <c r="R37" s="9"/>
-      <c r="S37" s="9"/>
-      <c r="T37" s="9"/>
-      <c r="U37" s="9"/>
-      <c r="V37" s="9"/>
-      <c r="W37" s="9"/>
-      <c r="X37" s="9"/>
-      <c r="Y37" s="9"/>
-      <c r="Z37" s="9"/>
+      <c r="C37" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F37" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H37" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="I37" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="J37" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="K37" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="L37" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="M37" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="N37" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="O37" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="P37" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q37" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="R37" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="S37" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="T37" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="U37" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="V37" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="W37" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="X37" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="Y37" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z37" s="25" t="s">
+        <v>214</v>
+      </c>
       <c r="AA37" s="8" t="s">
         <v>41</v>
       </c>
@@ -2008,30 +2587,78 @@
       <c r="B39" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="9"/>
-      <c r="N39" s="9"/>
-      <c r="O39" s="9"/>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="9"/>
-      <c r="R39" s="9"/>
-      <c r="S39" s="9"/>
-      <c r="T39" s="9"/>
-      <c r="U39" s="9"/>
-      <c r="V39" s="9"/>
-      <c r="W39" s="9"/>
-      <c r="X39" s="9"/>
-      <c r="Y39" s="9"/>
-      <c r="Z39" s="9"/>
+      <c r="C39" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F39" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H39" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="I39" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="J39" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="K39" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="L39" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="M39" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="N39" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="O39" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="P39" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q39" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="R39" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="S39" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="T39" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="U39" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="V39" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="W39" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="X39" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="Y39" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z39" s="25" t="s">
+        <v>226</v>
+      </c>
       <c r="AA39" s="8" t="s">
         <v>41</v>
       </c>
@@ -2120,33 +2747,77 @@
       <c r="B41" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
-      <c r="N41" s="9"/>
-      <c r="O41" s="9"/>
-      <c r="P41" s="9"/>
-      <c r="Q41" s="9"/>
-      <c r="R41" s="9"/>
-      <c r="S41" s="9"/>
-      <c r="T41" s="9"/>
-      <c r="U41" s="9"/>
-      <c r="V41" s="9"/>
-      <c r="W41" s="9"/>
-      <c r="X41" s="9"/>
+      <c r="C41" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F41" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H41" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="J41" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="K41" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="L41" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="M41" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="N41" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="O41" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="P41" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q41" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="R41" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="S41" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="T41" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="U41" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="V41" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="W41" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="X41" s="25" t="s">
+        <v>237</v>
+      </c>
       <c r="Y41" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="Z41" s="10" t="s">
-        <v>141</v>
+      <c r="Z41" s="25" t="s">
+        <v>238</v>
       </c>
       <c r="AA41" s="8" t="s">
         <v>41</v>
@@ -2325,35 +2996,83 @@
       <c r="B48" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
-      <c r="J48" s="9"/>
-      <c r="K48" s="9"/>
-      <c r="L48" s="9"/>
-      <c r="M48" s="9"/>
-      <c r="N48" s="9"/>
-      <c r="O48" s="9"/>
-      <c r="P48" s="9"/>
-      <c r="Q48" s="9"/>
-      <c r="R48" s="9"/>
-      <c r="S48" s="9"/>
-      <c r="T48" s="9"/>
-      <c r="U48" s="9"/>
-      <c r="V48" s="9"/>
-      <c r="W48" s="9"/>
-      <c r="X48" s="9"/>
-      <c r="Y48" s="9"/>
-      <c r="Z48" s="9"/>
+      <c r="C48" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="D48" s="9">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="E48" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="F48" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="G48" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="H48" s="9">
+        <v>0.112</v>
+      </c>
+      <c r="I48" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="J48" s="9">
+        <v>1.3</v>
+      </c>
+      <c r="K48" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="L48" s="9">
+        <v>2E-3</v>
+      </c>
+      <c r="M48" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="N48" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="O48" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="P48" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="Q48" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="R48" s="9">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="S48" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="T48" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="U48" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="V48" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="W48" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="X48" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="Y48" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="Z48" s="9">
+        <v>0.62</v>
+      </c>
       <c r="AA48" s="8">
         <v>450</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B49" s="6" t="s">
         <v>43</v>
       </c>
@@ -2433,39 +3152,87 @@
         <v>450</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B50" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9"/>
-      <c r="K50" s="9"/>
-      <c r="L50" s="9"/>
-      <c r="M50" s="9"/>
-      <c r="N50" s="9"/>
-      <c r="O50" s="9"/>
-      <c r="P50" s="9"/>
-      <c r="Q50" s="9"/>
-      <c r="R50" s="9"/>
-      <c r="S50" s="9"/>
-      <c r="T50" s="9"/>
-      <c r="U50" s="9"/>
-      <c r="V50" s="9"/>
-      <c r="W50" s="9"/>
-      <c r="X50" s="9"/>
-      <c r="Y50" s="9"/>
-      <c r="Z50" s="9"/>
+      <c r="C50" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="D50" s="9">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="E50" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="F50" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="G50" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="H50" s="9">
+        <v>0.112</v>
+      </c>
+      <c r="I50" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="J50" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="K50" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="L50" s="9">
+        <v>2E-3</v>
+      </c>
+      <c r="M50" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="N50" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="O50" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="P50" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="Q50" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="R50" s="9">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="S50" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="T50" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="U50" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="V50" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="W50" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="X50" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="Y50" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="Z50" s="9">
+        <v>0.62</v>
+      </c>
       <c r="AA50" s="8">
         <v>450</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B51" s="6" t="s">
         <v>57</v>
       </c>
@@ -2545,39 +3312,87 @@
         <v>450</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B52" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
-      <c r="J52" s="9"/>
-      <c r="K52" s="9"/>
-      <c r="L52" s="9"/>
-      <c r="M52" s="9"/>
-      <c r="N52" s="9"/>
-      <c r="O52" s="9"/>
-      <c r="P52" s="9"/>
-      <c r="Q52" s="9"/>
-      <c r="R52" s="9"/>
-      <c r="S52" s="9"/>
-      <c r="T52" s="9"/>
-      <c r="U52" s="9"/>
-      <c r="V52" s="9"/>
-      <c r="W52" s="9"/>
-      <c r="X52" s="9"/>
-      <c r="Y52" s="9"/>
-      <c r="Z52" s="9"/>
+      <c r="C52" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="D52" s="9">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="E52" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="F52" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="G52" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="H52" s="9">
+        <v>0.112</v>
+      </c>
+      <c r="I52" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="J52" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="K52" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="L52" s="9">
+        <v>2E-3</v>
+      </c>
+      <c r="M52" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="N52" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="O52" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="P52" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="Q52" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="R52" s="9">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="S52" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="T52" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="U52" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="V52" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="W52" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="X52" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="Y52" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="Z52" s="9">
+        <v>0.62</v>
+      </c>
       <c r="AA52" s="8">
         <v>450</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B53" s="6" t="s">
         <v>71</v>
       </c>
@@ -2657,39 +3472,87 @@
         <v>450</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B54" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="9"/>
-      <c r="K54" s="9"/>
-      <c r="L54" s="9"/>
-      <c r="M54" s="9"/>
-      <c r="N54" s="9"/>
-      <c r="O54" s="9"/>
-      <c r="P54" s="9"/>
-      <c r="Q54" s="9"/>
-      <c r="R54" s="9"/>
-      <c r="S54" s="9"/>
-      <c r="T54" s="9"/>
-      <c r="U54" s="9"/>
-      <c r="V54" s="9"/>
-      <c r="W54" s="9"/>
-      <c r="X54" s="9"/>
-      <c r="Y54" s="9"/>
-      <c r="Z54" s="9"/>
+      <c r="C54" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="D54" s="9">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="E54" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="F54" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="G54" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="H54" s="9">
+        <v>0.112</v>
+      </c>
+      <c r="I54" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="J54" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="K54" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="L54" s="9">
+        <v>2E-3</v>
+      </c>
+      <c r="M54" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="N54" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="O54" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="P54" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="Q54" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="R54" s="9">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="S54" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="T54" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="U54" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="V54" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="W54" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="X54" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="Y54" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="Z54" s="9">
+        <v>0.62</v>
+      </c>
       <c r="AA54" s="8">
         <v>450</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B55" s="6" t="s">
         <v>85</v>
       </c>
@@ -2769,39 +3632,87 @@
         <v>450</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B56" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="9"/>
-      <c r="J56" s="9"/>
-      <c r="K56" s="9"/>
-      <c r="L56" s="9"/>
-      <c r="M56" s="9"/>
-      <c r="N56" s="9"/>
-      <c r="O56" s="9"/>
-      <c r="P56" s="9"/>
-      <c r="Q56" s="9"/>
-      <c r="R56" s="9"/>
-      <c r="S56" s="9"/>
-      <c r="T56" s="9"/>
-      <c r="U56" s="9"/>
-      <c r="V56" s="9"/>
-      <c r="W56" s="9"/>
-      <c r="X56" s="9"/>
-      <c r="Y56" s="9"/>
-      <c r="Z56" s="9"/>
+      <c r="C56" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="D56" s="9">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="E56" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="F56" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="G56" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="H56" s="9">
+        <v>0.112</v>
+      </c>
+      <c r="I56" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="J56" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="K56" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="L56" s="9">
+        <v>2E-3</v>
+      </c>
+      <c r="M56" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="N56" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="O56" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="P56" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="Q56" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="R56" s="9">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="S56" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="T56" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="U56" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="V56" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="W56" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="X56" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="Y56" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="Z56" s="9">
+        <v>0.62</v>
+      </c>
       <c r="AA56" s="8">
         <v>450</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B57" s="6" t="s">
         <v>99</v>
       </c>
@@ -2881,39 +3792,87 @@
         <v>450</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B58" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
-      <c r="J58" s="9"/>
-      <c r="K58" s="9"/>
-      <c r="L58" s="9"/>
-      <c r="M58" s="9"/>
-      <c r="N58" s="9"/>
-      <c r="O58" s="9"/>
-      <c r="P58" s="9"/>
-      <c r="Q58" s="9"/>
-      <c r="R58" s="9"/>
-      <c r="S58" s="9"/>
-      <c r="T58" s="9"/>
-      <c r="U58" s="9"/>
-      <c r="V58" s="9"/>
-      <c r="W58" s="9"/>
-      <c r="X58" s="9"/>
-      <c r="Y58" s="9"/>
-      <c r="Z58" s="9"/>
+      <c r="C58" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="D58" s="9">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="E58" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="F58" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="G58" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="H58" s="9">
+        <v>0.112</v>
+      </c>
+      <c r="I58" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="J58" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="K58" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="L58" s="9">
+        <v>2E-3</v>
+      </c>
+      <c r="M58" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="N58" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="O58" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="P58" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="Q58" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="R58" s="9">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="S58" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="T58" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="U58" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="V58" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="W58" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="X58" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="Y58" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="Z58" s="9">
+        <v>0.62</v>
+      </c>
       <c r="AA58" s="8">
         <v>450</v>
       </c>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B59" s="6" t="s">
         <v>113</v>
       </c>
@@ -2993,39 +3952,87 @@
         <v>450</v>
       </c>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B60" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
-      <c r="J60" s="9"/>
-      <c r="K60" s="9"/>
-      <c r="L60" s="9"/>
-      <c r="M60" s="9"/>
-      <c r="N60" s="9"/>
-      <c r="O60" s="9"/>
-      <c r="P60" s="9"/>
-      <c r="Q60" s="9"/>
-      <c r="R60" s="9"/>
-      <c r="S60" s="9"/>
-      <c r="T60" s="9"/>
-      <c r="U60" s="9"/>
-      <c r="V60" s="9"/>
-      <c r="W60" s="9"/>
-      <c r="X60" s="9"/>
-      <c r="Y60" s="9"/>
-      <c r="Z60" s="9"/>
+      <c r="C60" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="D60" s="9">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="E60" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="F60" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="G60" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="H60" s="9">
+        <v>0.112</v>
+      </c>
+      <c r="I60" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="J60" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="K60" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="L60" s="9">
+        <v>2E-3</v>
+      </c>
+      <c r="M60" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="N60" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="O60" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="P60" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="Q60" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="R60" s="9">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="S60" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="T60" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="U60" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="V60" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="W60" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="X60" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="Y60" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="Z60" s="9">
+        <v>0.62</v>
+      </c>
       <c r="AA60" s="8">
         <v>450</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B61" s="6" t="s">
         <v>127</v>
       </c>
@@ -3105,1025 +4112,106 @@
         <v>450</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B62" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="9"/>
-      <c r="J62" s="9"/>
-      <c r="K62" s="9"/>
-      <c r="L62" s="9"/>
-      <c r="M62" s="9"/>
-      <c r="N62" s="9"/>
-      <c r="O62" s="9"/>
-      <c r="P62" s="9"/>
-      <c r="Q62" s="9"/>
-      <c r="R62" s="9"/>
-      <c r="S62" s="9"/>
-      <c r="T62" s="9"/>
-      <c r="U62" s="9"/>
-      <c r="V62" s="9"/>
-      <c r="W62" s="9"/>
-      <c r="X62" s="9"/>
+      <c r="C62" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="D62" s="9">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="E62" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="F62" s="9">
+        <v>0.113</v>
+      </c>
+      <c r="G62" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="H62" s="9">
+        <v>0.112</v>
+      </c>
+      <c r="I62" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="J62" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="K62" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="L62" s="9">
+        <v>2E-3</v>
+      </c>
+      <c r="M62" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="N62" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="O62" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="P62" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="Q62" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="R62" s="9">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="S62" s="12">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="T62" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="U62" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="V62" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="W62" s="11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="X62" s="9">
+        <v>0.4</v>
+      </c>
       <c r="Y62" s="11">
         <v>0.13100000000000001</v>
       </c>
-      <c r="Z62" s="12">
-        <v>0.24199999999999999</v>
+      <c r="Z62" s="9">
+        <v>0.62</v>
       </c>
       <c r="AA62" s="8">
         <v>450</v>
       </c>
     </row>
-    <row r="64" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B64" s="4"/>
-    </row>
-    <row r="66" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B66" s="5"/>
-      <c r="C66" s="6">
-        <v>1</v>
-      </c>
-      <c r="D66" s="6">
-        <v>2</v>
-      </c>
-      <c r="E66" s="6">
-        <v>3</v>
-      </c>
-      <c r="F66" s="6">
-        <v>4</v>
-      </c>
-      <c r="G66" s="6">
-        <v>5</v>
-      </c>
-      <c r="H66" s="6">
-        <v>6</v>
-      </c>
-      <c r="I66" s="6">
-        <v>7</v>
-      </c>
-      <c r="J66" s="6">
-        <v>8</v>
-      </c>
-      <c r="K66" s="6">
-        <v>9</v>
-      </c>
-      <c r="L66" s="6">
-        <v>10</v>
-      </c>
-      <c r="M66" s="6">
-        <v>11</v>
-      </c>
-      <c r="N66" s="6">
-        <v>12</v>
-      </c>
-      <c r="O66" s="6">
-        <v>13</v>
-      </c>
-      <c r="P66" s="6">
-        <v>14</v>
-      </c>
-      <c r="Q66" s="6">
-        <v>15</v>
-      </c>
-      <c r="R66" s="6">
-        <v>16</v>
-      </c>
-      <c r="S66" s="6">
-        <v>17</v>
-      </c>
-      <c r="T66" s="6">
-        <v>18</v>
-      </c>
-      <c r="U66" s="6">
-        <v>19</v>
-      </c>
-      <c r="V66" s="6">
-        <v>20</v>
-      </c>
-      <c r="W66" s="6">
-        <v>21</v>
-      </c>
-      <c r="X66" s="6">
-        <v>22</v>
-      </c>
-      <c r="Y66" s="6">
-        <v>23</v>
-      </c>
-      <c r="Z66" s="6">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="67" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B67" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C67" s="25">
-        <v>0.753</v>
-      </c>
-      <c r="D67" s="25">
-        <v>0.61599999999999999</v>
-      </c>
-      <c r="E67" s="25">
-        <v>0.92800000000000005</v>
-      </c>
-      <c r="F67" s="25">
-        <v>0.97199999999999998</v>
-      </c>
-      <c r="G67" s="25">
-        <v>0.83299999999999996</v>
-      </c>
-      <c r="H67" s="25">
-        <v>0.80800000000000005</v>
-      </c>
-      <c r="I67" s="25">
-        <v>0.91300000000000003</v>
-      </c>
-      <c r="J67" s="25">
-        <v>6.2</v>
-      </c>
-      <c r="K67" s="25">
-        <v>0.96799999999999997</v>
-      </c>
-      <c r="L67" s="25">
-        <v>0.92400000000000004</v>
-      </c>
-      <c r="M67" s="25">
-        <v>1.165</v>
-      </c>
-      <c r="N67" s="25">
-        <v>6.8330000000000002</v>
-      </c>
-      <c r="O67" s="25">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="P67" s="25">
-        <v>0.92800000000000005</v>
-      </c>
-      <c r="Q67" s="25">
-        <v>1.141</v>
-      </c>
-      <c r="R67" s="25">
-        <v>1.1279999999999999</v>
-      </c>
-      <c r="S67" s="25">
-        <v>1.2769999999999999</v>
-      </c>
-      <c r="T67" s="25">
-        <v>1.1559999999999999</v>
-      </c>
-      <c r="U67" s="25">
-        <v>0.72099999999999997</v>
-      </c>
-      <c r="V67" s="25">
-        <v>0.65700000000000003</v>
-      </c>
-      <c r="W67" s="25">
-        <v>0.96599999999999997</v>
-      </c>
-      <c r="X67" s="25">
-        <v>0.93200000000000005</v>
-      </c>
-      <c r="Y67" s="25">
-        <v>0.70799999999999996</v>
-      </c>
-      <c r="Z67" s="25">
-        <v>0.79500000000000004</v>
-      </c>
-      <c r="AA67" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="68" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B68" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="25"/>
-      <c r="G68" s="25"/>
-      <c r="H68" s="25"/>
-      <c r="I68" s="25"/>
-      <c r="J68" s="25"/>
-      <c r="K68" s="25"/>
-      <c r="L68" s="25"/>
-      <c r="M68" s="25"/>
-      <c r="N68" s="25"/>
-      <c r="O68" s="25"/>
-      <c r="P68" s="25"/>
-      <c r="Q68" s="25"/>
-      <c r="R68" s="25"/>
-      <c r="S68" s="25"/>
-      <c r="T68" s="25"/>
-      <c r="U68" s="25"/>
-      <c r="V68" s="25"/>
-      <c r="W68" s="25"/>
-      <c r="X68" s="25"/>
-      <c r="Y68" s="25"/>
-      <c r="Z68" s="25"/>
-      <c r="AA68" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="69" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B69" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C69" s="25">
-        <v>0.82299999999999995</v>
-      </c>
-      <c r="D69" s="25">
-        <v>0.89900000000000002</v>
-      </c>
-      <c r="E69" s="25">
-        <v>1.0609999999999999</v>
-      </c>
-      <c r="F69" s="25">
-        <v>1.002</v>
-      </c>
-      <c r="G69" s="25">
-        <v>5.4390000000000001</v>
-      </c>
-      <c r="H69" s="25">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="I69" s="25">
-        <v>0.96699999999999997</v>
-      </c>
-      <c r="J69" s="25">
-        <v>7.5289999999999999</v>
-      </c>
-      <c r="K69" s="25">
-        <v>6.7640000000000002</v>
-      </c>
-      <c r="L69" s="25">
-        <v>1.4319999999999999</v>
-      </c>
-      <c r="M69" s="25">
-        <v>0.79500000000000004</v>
-      </c>
-      <c r="N69" s="25">
-        <v>0.89700000000000002</v>
-      </c>
-      <c r="O69" s="25">
-        <v>1.875</v>
-      </c>
-      <c r="P69" s="25">
-        <v>2.4609999999999999</v>
-      </c>
-      <c r="Q69" s="25">
-        <v>3.569</v>
-      </c>
-      <c r="R69" s="25">
-        <v>3.3410000000000002</v>
-      </c>
-      <c r="S69" s="25">
-        <v>0.871</v>
-      </c>
-      <c r="T69" s="25">
-        <v>0.85</v>
-      </c>
-      <c r="U69" s="25">
-        <v>1.323</v>
-      </c>
-      <c r="V69" s="25">
-        <v>1.0549999999999999</v>
-      </c>
-      <c r="W69" s="25">
-        <v>1.085</v>
-      </c>
-      <c r="X69" s="25">
-        <v>0.95399999999999996</v>
-      </c>
-      <c r="Y69" s="25">
-        <v>1.147</v>
-      </c>
-      <c r="Z69" s="25">
-        <v>1.349</v>
-      </c>
-      <c r="AA69" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="70" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B70" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="25"/>
-      <c r="G70" s="25"/>
-      <c r="H70" s="25"/>
-      <c r="I70" s="25"/>
-      <c r="J70" s="25"/>
-      <c r="K70" s="25"/>
-      <c r="L70" s="25"/>
-      <c r="M70" s="25"/>
-      <c r="N70" s="25"/>
-      <c r="O70" s="25"/>
-      <c r="P70" s="25"/>
-      <c r="Q70" s="25"/>
-      <c r="R70" s="25"/>
-      <c r="S70" s="25"/>
-      <c r="T70" s="25"/>
-      <c r="U70" s="25"/>
-      <c r="V70" s="25"/>
-      <c r="W70" s="25"/>
-      <c r="X70" s="25"/>
-      <c r="Y70" s="25"/>
-      <c r="Z70" s="25"/>
-      <c r="AA70" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="71" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B71" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C71" s="25">
-        <v>1.23</v>
-      </c>
-      <c r="D71" s="25">
-        <v>6.9610000000000003</v>
-      </c>
-      <c r="E71" s="25">
-        <v>1.2430000000000001</v>
-      </c>
-      <c r="F71" s="25">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="G71" s="25">
-        <v>1.5840000000000001</v>
-      </c>
-      <c r="H71" s="25">
-        <v>1.609</v>
-      </c>
-      <c r="I71" s="25">
-        <v>5.6849999999999996</v>
-      </c>
-      <c r="J71" s="25">
-        <v>5.6440000000000001</v>
-      </c>
-      <c r="K71" s="25">
-        <v>0.88600000000000001</v>
-      </c>
-      <c r="L71" s="25">
-        <v>0.81399999999999995</v>
-      </c>
-      <c r="M71" s="25">
-        <v>1.077</v>
-      </c>
-      <c r="N71" s="25">
-        <v>1.095</v>
-      </c>
-      <c r="O71" s="25">
-        <v>1.03</v>
-      </c>
-      <c r="P71" s="25">
-        <v>1.129</v>
-      </c>
-      <c r="Q71" s="25">
-        <v>1.415</v>
-      </c>
-      <c r="R71" s="25">
-        <v>1.5429999999999999</v>
-      </c>
-      <c r="S71" s="25">
-        <v>0.752</v>
-      </c>
-      <c r="T71" s="25">
-        <v>0.70299999999999996</v>
-      </c>
-      <c r="U71" s="25">
-        <v>1.544</v>
-      </c>
-      <c r="V71" s="25">
-        <v>1.3560000000000001</v>
-      </c>
-      <c r="W71" s="25">
-        <v>0.999</v>
-      </c>
-      <c r="X71" s="25">
-        <v>3.976</v>
-      </c>
-      <c r="Y71" s="25">
-        <v>2.726</v>
-      </c>
-      <c r="Z71" s="25">
-        <v>2.863</v>
-      </c>
-      <c r="AA71" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="72" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B72" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C72" s="25"/>
-      <c r="D72" s="25"/>
-      <c r="E72" s="25"/>
-      <c r="F72" s="25"/>
-      <c r="G72" s="25"/>
-      <c r="H72" s="25"/>
-      <c r="I72" s="25"/>
-      <c r="J72" s="25"/>
-      <c r="K72" s="25"/>
-      <c r="L72" s="25"/>
-      <c r="M72" s="25"/>
-      <c r="N72" s="25"/>
-      <c r="O72" s="25"/>
-      <c r="P72" s="25"/>
-      <c r="Q72" s="25"/>
-      <c r="R72" s="25"/>
-      <c r="S72" s="25"/>
-      <c r="T72" s="25"/>
-      <c r="U72" s="25"/>
-      <c r="V72" s="25"/>
-      <c r="W72" s="25"/>
-      <c r="X72" s="25"/>
-      <c r="Y72" s="25"/>
-      <c r="Z72" s="25"/>
-      <c r="AA72" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="73" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B73" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C73" s="25">
-        <v>0.876</v>
-      </c>
-      <c r="D73" s="25">
-        <v>1.1060000000000001</v>
-      </c>
-      <c r="E73" s="25">
-        <v>1.014</v>
-      </c>
-      <c r="F73" s="25">
-        <v>0.92200000000000004</v>
-      </c>
-      <c r="G73" s="25">
-        <v>1.264</v>
-      </c>
-      <c r="H73" s="25">
-        <v>1.5389999999999999</v>
-      </c>
-      <c r="I73" s="25">
-        <v>1.387</v>
-      </c>
-      <c r="J73" s="25">
-        <v>1.238</v>
-      </c>
-      <c r="K73" s="25">
-        <v>1.38</v>
-      </c>
-      <c r="L73" s="25">
-        <v>1.53</v>
-      </c>
-      <c r="M73" s="25">
-        <v>1.53</v>
-      </c>
-      <c r="N73" s="25">
-        <v>1.518</v>
-      </c>
-      <c r="O73" s="25">
-        <v>2.1720000000000002</v>
-      </c>
-      <c r="P73" s="25">
-        <v>0.94099999999999995</v>
-      </c>
-      <c r="Q73" s="25">
-        <v>4.5220000000000002</v>
-      </c>
-      <c r="R73" s="25">
-        <v>5.1139999999999999</v>
-      </c>
-      <c r="S73" s="25">
-        <v>1.589</v>
-      </c>
-      <c r="T73" s="25">
-        <v>1.881</v>
-      </c>
-      <c r="U73" s="25">
-        <v>0.995</v>
-      </c>
-      <c r="V73" s="25">
-        <v>1.028</v>
-      </c>
-      <c r="W73" s="25">
-        <v>1.405</v>
-      </c>
-      <c r="X73" s="25">
-        <v>1.2669999999999999</v>
-      </c>
-      <c r="Y73" s="25">
-        <v>1.4550000000000001</v>
-      </c>
-      <c r="Z73" s="25">
-        <v>1.5229999999999999</v>
-      </c>
-      <c r="AA73" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="74" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B74" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C74" s="25"/>
-      <c r="D74" s="25"/>
-      <c r="E74" s="25"/>
-      <c r="F74" s="25"/>
-      <c r="G74" s="25"/>
-      <c r="H74" s="25"/>
-      <c r="I74" s="25"/>
-      <c r="J74" s="25"/>
-      <c r="K74" s="25"/>
-      <c r="L74" s="25"/>
-      <c r="M74" s="25"/>
-      <c r="N74" s="25"/>
-      <c r="O74" s="25"/>
-      <c r="P74" s="25"/>
-      <c r="Q74" s="25"/>
-      <c r="R74" s="25"/>
-      <c r="S74" s="25"/>
-      <c r="T74" s="25"/>
-      <c r="U74" s="25"/>
-      <c r="V74" s="25"/>
-      <c r="W74" s="25"/>
-      <c r="X74" s="25"/>
-      <c r="Y74" s="25"/>
-      <c r="Z74" s="25"/>
-      <c r="AA74" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="75" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B75" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C75" s="25">
-        <v>0.71299999999999997</v>
-      </c>
-      <c r="D75" s="25">
-        <v>0.71699999999999997</v>
-      </c>
-      <c r="E75" s="25">
-        <v>0.92100000000000004</v>
-      </c>
-      <c r="F75" s="25">
-        <v>0.90900000000000003</v>
-      </c>
-      <c r="G75" s="25">
-        <v>1.7410000000000001</v>
-      </c>
-      <c r="H75" s="25">
-        <v>1.698</v>
-      </c>
-      <c r="I75" s="25">
-        <v>1.107</v>
-      </c>
-      <c r="J75" s="25">
-        <v>1.2330000000000001</v>
-      </c>
-      <c r="K75" s="25">
-        <v>3.2360000000000002</v>
-      </c>
-      <c r="L75" s="25">
-        <v>1.4059999999999999</v>
-      </c>
-      <c r="M75" s="25">
-        <v>2.5579999999999998</v>
-      </c>
-      <c r="N75" s="25">
-        <v>1.1020000000000001</v>
-      </c>
-      <c r="O75" s="25">
-        <v>1.3520000000000001</v>
-      </c>
-      <c r="P75" s="25">
-        <v>1.4139999999999999</v>
-      </c>
-      <c r="Q75" s="25">
-        <v>1.25</v>
-      </c>
-      <c r="R75" s="25">
-        <v>0.97</v>
-      </c>
-      <c r="S75" s="25">
-        <v>5.1349999999999998</v>
-      </c>
-      <c r="T75" s="25">
-        <v>1.5049999999999999</v>
-      </c>
-      <c r="U75" s="25">
-        <v>10.113</v>
-      </c>
-      <c r="V75" s="25">
-        <v>1.6879999999999999</v>
-      </c>
-      <c r="W75" s="25">
-        <v>0.83099999999999996</v>
-      </c>
-      <c r="X75" s="25">
-        <v>0.75600000000000001</v>
-      </c>
-      <c r="Y75" s="25">
-        <v>1.542</v>
-      </c>
-      <c r="Z75" s="25">
-        <v>1.3109999999999999</v>
-      </c>
-      <c r="AA75" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="76" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B76" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C76" s="25"/>
-      <c r="D76" s="25"/>
-      <c r="E76" s="25"/>
-      <c r="F76" s="25"/>
-      <c r="G76" s="25"/>
-      <c r="H76" s="25"/>
-      <c r="I76" s="25"/>
-      <c r="J76" s="25"/>
-      <c r="K76" s="25"/>
-      <c r="L76" s="25"/>
-      <c r="M76" s="25"/>
-      <c r="N76" s="25"/>
-      <c r="O76" s="25"/>
-      <c r="P76" s="25"/>
-      <c r="Q76" s="25"/>
-      <c r="R76" s="25"/>
-      <c r="S76" s="25"/>
-      <c r="T76" s="25"/>
-      <c r="U76" s="25"/>
-      <c r="V76" s="25"/>
-      <c r="W76" s="25"/>
-      <c r="X76" s="25"/>
-      <c r="Y76" s="25"/>
-      <c r="Z76" s="25"/>
-      <c r="AA76" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="77" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B77" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C77" s="25">
-        <v>0.95699999999999996</v>
-      </c>
-      <c r="D77" s="25">
-        <v>1.046</v>
-      </c>
-      <c r="E77" s="25">
-        <v>1.1679999999999999</v>
-      </c>
-      <c r="F77" s="25">
-        <v>1.1679999999999999</v>
-      </c>
-      <c r="G77" s="25">
-        <v>0.97099999999999997</v>
-      </c>
-      <c r="H77" s="25">
-        <v>0.998</v>
-      </c>
-      <c r="I77" s="25">
-        <v>0.71799999999999997</v>
-      </c>
-      <c r="J77" s="25">
-        <v>3.3250000000000002</v>
-      </c>
-      <c r="K77" s="25">
-        <v>1.087</v>
-      </c>
-      <c r="L77" s="25">
-        <v>1.462</v>
-      </c>
-      <c r="M77" s="25">
-        <v>0.874</v>
-      </c>
-      <c r="N77" s="25">
-        <v>1.06</v>
-      </c>
-      <c r="O77" s="25">
-        <v>8.7260000000000009</v>
-      </c>
-      <c r="P77" s="25">
-        <v>8.5939999999999994</v>
-      </c>
-      <c r="Q77" s="25">
-        <v>1.3089999999999999</v>
-      </c>
-      <c r="R77" s="25">
-        <v>4.5250000000000004</v>
-      </c>
-      <c r="S77" s="25">
-        <v>1.1659999999999999</v>
-      </c>
-      <c r="T77" s="25">
-        <v>1.1259999999999999</v>
-      </c>
-      <c r="U77" s="25">
-        <v>2.7890000000000001</v>
-      </c>
-      <c r="V77" s="25">
-        <v>2.8239999999999998</v>
-      </c>
-      <c r="W77" s="25">
-        <v>1.0249999999999999</v>
-      </c>
-      <c r="X77" s="25">
-        <v>1.222</v>
-      </c>
-      <c r="Y77" s="25">
-        <v>1.5109999999999999</v>
-      </c>
-      <c r="Z77" s="25">
-        <v>1.6140000000000001</v>
-      </c>
-      <c r="AA77" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="78" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B78" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C78" s="25"/>
-      <c r="D78" s="25"/>
-      <c r="E78" s="25"/>
-      <c r="F78" s="25"/>
-      <c r="G78" s="25"/>
-      <c r="H78" s="25"/>
-      <c r="I78" s="25"/>
-      <c r="J78" s="25"/>
-      <c r="K78" s="25"/>
-      <c r="L78" s="25"/>
-      <c r="M78" s="25"/>
-      <c r="N78" s="25"/>
-      <c r="O78" s="25"/>
-      <c r="P78" s="25"/>
-      <c r="Q78" s="25"/>
-      <c r="R78" s="25"/>
-      <c r="S78" s="25"/>
-      <c r="T78" s="25"/>
-      <c r="U78" s="25"/>
-      <c r="V78" s="25"/>
-      <c r="W78" s="25"/>
-      <c r="X78" s="25"/>
-      <c r="Y78" s="25"/>
-      <c r="Z78" s="25"/>
-      <c r="AA78" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="79" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B79" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C79" s="25">
-        <v>1.2</v>
-      </c>
-      <c r="D79" s="25">
-        <v>1.343</v>
-      </c>
-      <c r="E79" s="25">
-        <v>1.0489999999999999</v>
-      </c>
-      <c r="F79" s="25">
-        <v>0.99</v>
-      </c>
-      <c r="G79" s="25">
-        <v>1.145</v>
-      </c>
-      <c r="H79" s="25">
-        <v>8.5649999999999995</v>
-      </c>
-      <c r="I79" s="25">
-        <v>0.75700000000000001</v>
-      </c>
-      <c r="J79" s="25">
-        <v>0.87</v>
-      </c>
-      <c r="K79" s="25">
-        <v>2.6389999999999998</v>
-      </c>
-      <c r="L79" s="25">
-        <v>1.2729999999999999</v>
-      </c>
-      <c r="M79" s="25">
-        <v>1.665</v>
-      </c>
-      <c r="N79" s="25">
-        <v>2.089</v>
-      </c>
-      <c r="O79" s="25">
-        <v>0.95399999999999996</v>
-      </c>
-      <c r="P79" s="25">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="Q79" s="25">
-        <v>0.68200000000000005</v>
-      </c>
-      <c r="R79" s="25">
-        <v>0.95799999999999996</v>
-      </c>
-      <c r="S79" s="25">
-        <v>1.1619999999999999</v>
-      </c>
-      <c r="T79" s="25">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="U79" s="25">
-        <v>3.153</v>
-      </c>
-      <c r="V79" s="25">
-        <v>0.74199999999999999</v>
-      </c>
-      <c r="W79" s="25">
-        <v>5.8570000000000002</v>
-      </c>
-      <c r="X79" s="25">
-        <v>1.579</v>
-      </c>
-      <c r="Y79" s="25">
-        <v>1.169</v>
-      </c>
-      <c r="Z79" s="25">
-        <v>1.069</v>
-      </c>
-      <c r="AA79" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="80" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B80" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C80" s="25"/>
-      <c r="D80" s="25"/>
-      <c r="E80" s="25"/>
-      <c r="F80" s="25"/>
-      <c r="G80" s="25"/>
-      <c r="H80" s="25"/>
-      <c r="I80" s="25"/>
-      <c r="J80" s="25"/>
-      <c r="K80" s="25"/>
-      <c r="L80" s="25"/>
-      <c r="M80" s="25"/>
-      <c r="N80" s="25"/>
-      <c r="O80" s="25"/>
-      <c r="P80" s="25"/>
-      <c r="Q80" s="25"/>
-      <c r="R80" s="25"/>
-      <c r="S80" s="25"/>
-      <c r="T80" s="25"/>
-      <c r="U80" s="25"/>
-      <c r="V80" s="25"/>
-      <c r="W80" s="25"/>
-      <c r="X80" s="25"/>
-      <c r="Y80" s="25"/>
-      <c r="Z80" s="25"/>
-      <c r="AA80" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="81" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B81" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C81" s="25">
-        <v>1.08</v>
-      </c>
-      <c r="D81" s="25">
-        <v>4.4950000000000001</v>
-      </c>
-      <c r="E81" s="25">
-        <v>1.581</v>
-      </c>
-      <c r="F81" s="25">
-        <v>1.5780000000000001</v>
-      </c>
-      <c r="G81" s="25">
-        <v>0.879</v>
-      </c>
-      <c r="H81" s="25">
-        <v>0.79200000000000004</v>
-      </c>
-      <c r="I81" s="25">
-        <v>0.89800000000000002</v>
-      </c>
-      <c r="J81" s="25">
-        <v>1.022</v>
-      </c>
-      <c r="K81" s="25">
-        <v>0.92400000000000004</v>
-      </c>
-      <c r="L81" s="25">
-        <v>0.9</v>
-      </c>
-      <c r="M81" s="25">
-        <v>2.371</v>
-      </c>
-      <c r="N81" s="25">
-        <v>1.8919999999999999</v>
-      </c>
-      <c r="O81" s="25">
-        <v>1.034</v>
-      </c>
-      <c r="P81" s="25">
-        <v>0.92800000000000005</v>
-      </c>
-      <c r="Q81" s="25">
-        <v>0.94899999999999995</v>
-      </c>
-      <c r="R81" s="25">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="S81" s="25">
-        <v>0.98299999999999998</v>
-      </c>
-      <c r="T81" s="25">
-        <v>0.93500000000000005</v>
-      </c>
-      <c r="U81" s="25">
-        <v>0.97399999999999998</v>
-      </c>
-      <c r="V81" s="25">
-        <v>1.4490000000000001</v>
-      </c>
-      <c r="W81" s="25">
-        <v>1.268</v>
-      </c>
-      <c r="X81" s="25">
-        <v>1.474</v>
-      </c>
-      <c r="Y81" s="25">
-        <v>3.4449999999999998</v>
-      </c>
-      <c r="Z81" s="25">
-        <v>2.0110000000000001</v>
-      </c>
-      <c r="AA81" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="82" spans="2:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="B82" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C82" s="25"/>
-      <c r="D82" s="25"/>
-      <c r="E82" s="25"/>
-      <c r="F82" s="25"/>
-      <c r="G82" s="25"/>
-      <c r="H82" s="25"/>
-      <c r="I82" s="25"/>
-      <c r="J82" s="25"/>
-      <c r="K82" s="25"/>
-      <c r="L82" s="25"/>
-      <c r="M82" s="25"/>
-      <c r="N82" s="25"/>
-      <c r="O82" s="25"/>
-      <c r="P82" s="25"/>
-      <c r="Q82" s="25"/>
-      <c r="R82" s="25"/>
-      <c r="S82" s="25"/>
-      <c r="T82" s="25"/>
-      <c r="U82" s="25"/>
-      <c r="V82" s="25"/>
-      <c r="W82" s="25"/>
-      <c r="X82" s="25"/>
-      <c r="Y82" s="25">
-        <v>0.70399999999999996</v>
-      </c>
-      <c r="Z82" s="25">
-        <v>1.296</v>
-      </c>
-      <c r="AA82" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
+  <conditionalFormatting sqref="C47:Z62">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color theme="4" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>